<commit_message>
Update validation: check exits employee
</commit_message>
<xml_diff>
--- a/ITGlobalProject/Content/FileUpload/DanhSachNhanVien-Import.xlsx
+++ b/ITGlobalProject/Content/FileUpload/DanhSachNhanVien-Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnguy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E35CE-508A-4E03-91B8-2E0028CA9E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9978C31A-6CAC-4873-9E10-AA49BD0609DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18360" yWindow="3210" windowWidth="16095" windowHeight="14370" xr2:uid="{D863059B-1735-4B2D-BB81-759A3D9E481F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D863059B-1735-4B2D-BB81-759A3D9E481F}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông Tin" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>STT</t>
   </si>
@@ -106,13 +106,7 @@
     <t>Nhân viên chính thức</t>
   </si>
   <si>
-    <t>Front-End Developer</t>
-  </si>
-  <si>
     <t>Back-End Developer</t>
-  </si>
-  <si>
-    <t>Full-Stack Developer</t>
   </si>
   <si>
     <t>Business Analyst</t>
@@ -149,13 +143,19 @@
     </r>
   </si>
   <si>
-    <t>Lê Thành Khang'</t>
-  </si>
-  <si>
     <t>2000-10-30</t>
   </si>
   <si>
     <t>2022-06-12</t>
+  </si>
+  <si>
+    <t>Đặng Văn Tuấn</t>
+  </si>
+  <si>
+    <t>Front-End-Developer</t>
+  </si>
+  <si>
+    <t>Full-Stack Development</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,6 +453,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -464,21 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1004,8 +1007,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}" name="Table4" displayName="Table4" ref="A2:M18" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A2:M18" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}" name="Table4" displayName="Table4" ref="A2:M5" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="A2:M5" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{BD8030A3-5E0B-43AD-8C5A-13ACC4A69AFB}" name="STT" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{B7CC9FE9-4234-4AE1-87BF-F151D48C284C}" name="Họ và Tên" dataDxfId="19"/>
@@ -1334,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55C3C43-D4B0-4F2A-9605-24C832C66003}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,21 +1361,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="A1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -1403,10 +1406,10 @@
         <v>5</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L2" s="22" t="s">
         <v>13</v>
@@ -1427,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>8</v>
@@ -1445,10 +1448,10 @@
         <v>30000000</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M3" s="19" t="s">
         <v>20</v>
@@ -1461,24 +1464,18 @@
       <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>8</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1486,586 +1483,47 @@
         <v>30000000</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M4" s="19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="30">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="29" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="29" t="s">
+      <c r="E5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="29" t="s">
+      <c r="H5" s="27"/>
+      <c r="I5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="28">
         <v>30000000</v>
       </c>
-      <c r="K5" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
-        <v>4</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
-        <v>5</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K7" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
-        <v>6</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L8" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>7</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
-        <v>8</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
-        <v>9</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
-        <v>10</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
-        <v>11</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K13" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L13" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
-        <v>12</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K14" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
-        <v>13</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K15" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L15" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
-        <v>14</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K16" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L16" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
-        <v>15</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="32">
-        <v>30000000</v>
-      </c>
-      <c r="K18" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L18" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M18" s="33" t="s">
+      <c r="K5" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="29" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2075,41 +1533,26 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G18" xr:uid="{866CB8C6-8ADA-4E03-97B3-A9A4C8B05E59}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G5" xr:uid="{866CB8C6-8ADA-4E03-97B3-A9A4C8B05E59}">
       <formula1>"Nam,Nữ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I18" xr:uid="{02E7F330-C014-4C13-BE42-7BD894338365}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I5" xr:uid="{02E7F330-C014-4C13-BE42-7BD894338365}">
       <formula1>"Độc thân,Đã kết hôn,Khác"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M18" xr:uid="{37061D6D-240A-4825-9558-8E20E1AB1D7D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M5" xr:uid="{37061D6D-240A-4825-9558-8E20E1AB1D7D}">
       <formula1>"Thực tập sinh,Thử việc,Nhân viên chính thức"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L18" xr:uid="{473363A2-96C3-48E0-A81E-BBB7A510E3D1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L5" xr:uid="{473363A2-96C3-48E0-A81E-BBB7A510E3D1}">
       <formula1>Chucdanh</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" xr:uid="{CC7C0DCE-74A9-4099-8658-1C9C59A5BD79}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{317F0368-1F8C-4218-9D4C-87951E4D3F14}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{FE5FBDE8-9423-406F-B306-4CD545C705F1}"/>
-    <hyperlink ref="H6" r:id="rId4" xr:uid="{9EA80602-A299-4470-9F9D-5076E529714B}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{474A50C9-01F9-4E32-89EA-D2075307EF19}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{78C6F559-E3E7-4148-9FA2-5FD4035DAD5E}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{FAEFB254-945D-4837-A9FE-699BE2F4CA95}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{E6864FC4-5D10-41DC-82B2-F2873E91CBF1}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{B388EB5B-4615-4E9D-A148-3896021EBF14}"/>
-    <hyperlink ref="H12" r:id="rId10" xr:uid="{F9B60780-20CC-4FCB-BAB1-EE96314D90FC}"/>
-    <hyperlink ref="H13" r:id="rId11" xr:uid="{8D390E52-CAC2-4B14-91FB-46DB2ED2A833}"/>
-    <hyperlink ref="H14" r:id="rId12" xr:uid="{8C31DA5B-A5BB-4256-8CB5-E098E3D5FFB0}"/>
-    <hyperlink ref="H15" r:id="rId13" xr:uid="{63EFB53A-9874-47A9-B3A7-2017DB99EDB4}"/>
-    <hyperlink ref="H16" r:id="rId14" xr:uid="{1ED73EE4-DA0D-4C2D-893B-57881B238855}"/>
-    <hyperlink ref="H17" r:id="rId15" xr:uid="{6265B2A9-8AA5-482E-9297-3160DDA4640B}"/>
-    <hyperlink ref="H18" r:id="rId16" xr:uid="{7C97841D-E862-4985-AEA4-C5C21A281057}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2119,7 +1562,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,11 +1573,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2152,10 +1595,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2163,10 +1606,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2174,10 +1617,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2185,10 +1628,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2196,10 +1639,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update function: import imployee
</commit_message>
<xml_diff>
--- a/ITGlobalProject/Content/FileUpload/DanhSachNhanVien-Import.xlsx
+++ b/ITGlobalProject/Content/FileUpload/DanhSachNhanVien-Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnguy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9978C31A-6CAC-4873-9E10-AA49BD0609DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E35CE-508A-4E03-91B8-2E0028CA9E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D863059B-1735-4B2D-BB81-759A3D9E481F}"/>
+    <workbookView xWindow="18360" yWindow="3210" windowWidth="16095" windowHeight="14370" xr2:uid="{D863059B-1735-4B2D-BB81-759A3D9E481F}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông Tin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="Chucdanh">Table3[Tên chức danh]</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,90 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>Họ và Tên</t>
-  </si>
-  <si>
-    <t>CMND/CCCD</t>
-  </si>
-  <si>
-    <t>Quốc tịch</t>
-  </si>
-  <si>
-    <t>Giới tính</t>
-  </si>
-  <si>
-    <t>Hôn nhân</t>
-  </si>
-  <si>
-    <t>Việt Nam</t>
-  </si>
-  <si>
-    <t>070288372732</t>
-  </si>
-  <si>
-    <t>0367909248</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
-    <t>Tên chức danh</t>
-  </si>
-  <si>
-    <t>Tên bộ phận</t>
-  </si>
-  <si>
-    <t>DANH SÁCH CHỨC DANH</t>
-  </si>
-  <si>
-    <t>Chức danh</t>
-  </si>
-  <si>
-    <t>Hình thức làm việc</t>
-  </si>
-  <si>
-    <t>Ngày sinh 
-(yyyy-MM-dd)</t>
-  </si>
-  <si>
-    <t>Số điện thoại</t>
-  </si>
-  <si>
-    <t>Độc thân</t>
-  </si>
-  <si>
-    <t>địa chỉ Email Công ty</t>
-  </si>
-  <si>
-    <t>tuan.197pm21996@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>Nhân viên chính thức</t>
-  </si>
-  <si>
-    <t>Back-End Developer</t>
-  </si>
-  <si>
-    <t>Business Analyst</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>Phát triển phần mềm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ngày vào làm
-(yyyy-MM-dd) </t>
-  </si>
-  <si>
-    <t>Mức lương (VND)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="33">
   <si>
     <r>
       <t xml:space="preserve">DANH SÁCH NHÂN VIÊN
@@ -143,19 +60,102 @@
     </r>
   </si>
   <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Họ và Tên</t>
+  </si>
+  <si>
+    <t>CMND/CCCD</t>
+  </si>
+  <si>
+    <t>Quốc tịch</t>
+  </si>
+  <si>
+    <t>Ngày sinh 
+(yyyy-MM-dd)</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>địa chỉ Email Công ty</t>
+  </si>
+  <si>
+    <t>Hôn nhân</t>
+  </si>
+  <si>
+    <t>Mức lương (VND)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày vào làm
+(yyyy-MM-dd) </t>
+  </si>
+  <si>
+    <t>Chức danh</t>
+  </si>
+  <si>
+    <t>Hình thức làm việc</t>
+  </si>
+  <si>
+    <t>070288372732</t>
+  </si>
+  <si>
+    <t>Việt Nam</t>
+  </si>
+  <si>
     <t>2000-10-30</t>
   </si>
   <si>
+    <t>0367909248</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>tuan.197pm21996@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>Độc thân</t>
+  </si>
+  <si>
     <t>2022-06-12</t>
   </si>
   <si>
-    <t>Đặng Văn Tuấn</t>
-  </si>
-  <si>
-    <t>Front-End-Developer</t>
-  </si>
-  <si>
-    <t>Full-Stack Development</t>
+    <t>Full-Stack Developer</t>
+  </si>
+  <si>
+    <t>Nhân viên chính thức</t>
+  </si>
+  <si>
+    <t>Lê Thành Khang'</t>
+  </si>
+  <si>
+    <t>DANH SÁCH CHỨC DANH</t>
+  </si>
+  <si>
+    <t>Tên chức danh</t>
+  </si>
+  <si>
+    <t>Tên bộ phận</t>
+  </si>
+  <si>
+    <t>Front-End Developer</t>
+  </si>
+  <si>
+    <t>Phát triển phần mềm</t>
+  </si>
+  <si>
+    <t>Back-End Developer</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
@@ -166,7 +166,7 @@
     <numFmt numFmtId="164" formatCode="#,##0\ _₫"/>
     <numFmt numFmtId="165" formatCode="[&lt;=999999][$-1000000]###\-###;[$-1000000]\(##\)\ ###\-###"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,9 +468,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -485,8 +482,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
     <dxf>
@@ -610,6 +607,13 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -638,13 +642,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -935,6 +932,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -944,13 +948,6 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1007,8 +1004,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}" name="Table4" displayName="Table4" ref="A2:M5" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A2:M5" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}" name="Table4" displayName="Table4" ref="A2:M18" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
+  <autoFilter ref="A2:M18" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{BD8030A3-5E0B-43AD-8C5A-13ACC4A69AFB}" name="STT" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{B7CC9FE9-4234-4AE1-87BF-F151D48C284C}" name="Họ và Tên" dataDxfId="19"/>
@@ -1029,7 +1026,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6A2D9191-4CE9-4E69-B805-9A4FDC6A0840}" name="Table3" displayName="Table3" ref="A2:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6A2D9191-4CE9-4E69-B805-9A4FDC6A0840}" name="Table3" displayName="Table3" ref="A2:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
   <autoFilter ref="A2:C7" xr:uid="{6A2D9191-4CE9-4E69-B805-9A4FDC6A0840}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D2BE2BAF-1CF2-404E-A970-E88DD633B934}" name="STT" dataDxfId="2"/>
@@ -1041,7 +1038,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1337,13 +1334,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55C3C43-D4B0-4F2A-9605-24C832C66003}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -1360,171 +1357,716 @@
     <col min="13" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-    </row>
-    <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="43.5" customHeight="1">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" ht="30.75" customHeight="1">
       <c r="A2" s="20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="L2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="18">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J3" s="7">
         <v>30000000</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="18">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="G4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="I4" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J4" s="7">
         <v>30000000</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="18">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
-        <v>3</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="25" t="s">
-        <v>17</v>
       </c>
       <c r="J5" s="28">
         <v>30000000</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="L5" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="18">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="L6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="18">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="25" t="s">
         <v>20</v>
+      </c>
+      <c r="J7" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="18">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="18">
+        <v>7</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="18">
+        <v>8</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="18">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="18">
+        <v>10</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="18">
+        <v>11</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="18">
+        <v>12</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="18">
+        <v>13</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="18">
+        <v>14</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="18">
+        <v>15</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="28">
+        <v>30000000</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="29" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1533,26 +2075,41 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G5" xr:uid="{866CB8C6-8ADA-4E03-97B3-A9A4C8B05E59}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G18" xr:uid="{866CB8C6-8ADA-4E03-97B3-A9A4C8B05E59}">
       <formula1>"Nam,Nữ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I5" xr:uid="{02E7F330-C014-4C13-BE42-7BD894338365}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I18" xr:uid="{02E7F330-C014-4C13-BE42-7BD894338365}">
       <formula1>"Độc thân,Đã kết hôn,Khác"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M5" xr:uid="{37061D6D-240A-4825-9558-8E20E1AB1D7D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M18" xr:uid="{37061D6D-240A-4825-9558-8E20E1AB1D7D}">
       <formula1>"Thực tập sinh,Thử việc,Nhân viên chính thức"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L5" xr:uid="{473363A2-96C3-48E0-A81E-BBB7A510E3D1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L18" xr:uid="{473363A2-96C3-48E0-A81E-BBB7A510E3D1}">
       <formula1>Chucdanh</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" xr:uid="{CC7C0DCE-74A9-4099-8658-1C9C59A5BD79}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{317F0368-1F8C-4218-9D4C-87951E4D3F14}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{FE5FBDE8-9423-406F-B306-4CD545C705F1}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{9EA80602-A299-4470-9F9D-5076E529714B}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{474A50C9-01F9-4E32-89EA-D2075307EF19}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{78C6F559-E3E7-4148-9FA2-5FD4035DAD5E}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{FAEFB254-945D-4837-A9FE-699BE2F4CA95}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{E6864FC4-5D10-41DC-82B2-F2873E91CBF1}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{B388EB5B-4615-4E9D-A148-3896021EBF14}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{F9B60780-20CC-4FCB-BAB1-EE96314D90FC}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{8D390E52-CAC2-4B14-91FB-46DB2ED2A833}"/>
+    <hyperlink ref="H14" r:id="rId12" xr:uid="{8C31DA5B-A5BB-4256-8CB5-E098E3D5FFB0}"/>
+    <hyperlink ref="H15" r:id="rId13" xr:uid="{63EFB53A-9874-47A9-B3A7-2017DB99EDB4}"/>
+    <hyperlink ref="H16" r:id="rId14" xr:uid="{1ED73EE4-DA0D-4C2D-893B-57881B238855}"/>
+    <hyperlink ref="H17" r:id="rId15" xr:uid="{6265B2A9-8AA5-482E-9297-3160DDA4640B}"/>
+    <hyperlink ref="H18" r:id="rId16" xr:uid="{7C97841D-E862-4985-AEA4-C5C21A281057}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1562,87 +2119,87 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A1" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="33"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="15">
         <v>7</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update function: view detail payroll
</commit_message>
<xml_diff>
--- a/ITGlobalProject/Content/FileUpload/DanhSachNhanVien-Import.xlsx
+++ b/ITGlobalProject/Content/FileUpload/DanhSachNhanVien-Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnguy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanlangunivn-my.sharepoint.com/personal/loi_197pm09475_vanlanguni_vn/Documents/CAPSTONE 2022/CAPSTONE - Team 06/6. Others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E35CE-508A-4E03-91B8-2E0028CA9E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{393E35CE-508A-4E03-91B8-2E0028CA9E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46EA78A8-0BC7-4C10-BDC1-3762A541C499}"/>
   <bookViews>
-    <workbookView xWindow="18360" yWindow="3210" windowWidth="16095" windowHeight="14370" xr2:uid="{D863059B-1735-4B2D-BB81-759A3D9E481F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D863059B-1735-4B2D-BB81-759A3D9E481F}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông Tin" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="45">
   <si>
     <r>
       <t xml:space="preserve">DANH SÁCH NHÂN VIÊN
@@ -52,7 +52,7 @@
         <u/>
         <sz val="10"/>
         <color theme="0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -82,7 +82,7 @@
     <t>Giới tính</t>
   </si>
   <si>
-    <t>địa chỉ Email Công ty</t>
+    <t>Địa chỉ Email Công ty</t>
   </si>
   <si>
     <t>Hôn nhân</t>
@@ -116,7 +116,7 @@
     <t>Nam</t>
   </si>
   <si>
-    <t>tuan.197pm21996@vanlanguni.vn</t>
+    <t>khang.197pm21936@vanlanguni.vn</t>
   </si>
   <si>
     <t>Độc thân</t>
@@ -131,9 +131,39 @@
     <t>Nhân viên chính thức</t>
   </si>
   <si>
+    <t>070288372312</t>
+  </si>
+  <si>
+    <t>0367909241</t>
+  </si>
+  <si>
+    <t>nhan.197pm21926@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Huy Hoàng</t>
+  </si>
+  <si>
+    <t>070288372821</t>
+  </si>
+  <si>
+    <t>0367909242</t>
+  </si>
+  <si>
+    <t>hoang.197pm21936@vanlanguni.vn</t>
+  </si>
+  <si>
     <t>Lê Thành Khang'</t>
   </si>
   <si>
+    <t>tuan.197pm21936@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>036790924</t>
+  </si>
+  <si>
+    <t>0702883722</t>
+  </si>
+  <si>
     <t>DANH SÁCH CHỨC DANH</t>
   </si>
   <si>
@@ -156,6 +186,12 @@
   </si>
   <si>
     <t>Tester</t>
+  </si>
+  <si>
+    <t>Nguyễn Hiếu Nhân,</t>
+  </si>
+  <si>
+    <t>Lê Tuấn Khang,</t>
   </si>
 </sst>
 </file>
@@ -166,18 +202,18 @@
     <numFmt numFmtId="164" formatCode="#,##0\ _₫"/>
     <numFmt numFmtId="165" formatCode="[&lt;=999999][$-1000000]###\-###;[$-1000000]\(##\)\ ###\-###"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -185,7 +221,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -193,13 +229,13 @@
       <b/>
       <sz val="13"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -208,7 +244,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -216,7 +252,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -225,7 +261,7 @@
       <u/>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -383,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,9 +495,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -482,8 +515,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="25">
     <dxf>
@@ -607,13 +640,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -642,6 +668,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -932,13 +965,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -948,6 +974,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1004,7 +1037,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}" name="Table4" displayName="Table4" ref="A2:M18" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}" name="Table4" displayName="Table4" ref="A2:M18" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A2:M18" xr:uid="{AB9EF11F-0F98-4C6F-8F92-9C38C4F4C534}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{BD8030A3-5E0B-43AD-8C5A-13ACC4A69AFB}" name="STT" dataDxfId="20"/>
@@ -1014,7 +1047,7 @@
     <tableColumn id="5" xr3:uid="{F83E2F7F-8A9C-4D02-9926-D5AE40EE0DC7}" name="Ngày sinh _x000a_(yyyy-MM-dd)" dataDxfId="16"/>
     <tableColumn id="6" xr3:uid="{D6BDA48C-AF13-4001-AE5A-E1B667C94FCA}" name="Số điện thoại" dataDxfId="15"/>
     <tableColumn id="7" xr3:uid="{10689818-E465-4235-83E1-7B4A2C4D2524}" name="Giới tính" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{58007B10-36BE-44AC-A799-F5EF9271B1B1}" name="địa chỉ Email Công ty" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{58007B10-36BE-44AC-A799-F5EF9271B1B1}" name="Địa chỉ Email Công ty" dataDxfId="13"/>
     <tableColumn id="9" xr3:uid="{A45F40B3-F1E4-4D0A-A8F7-FDFB2F19659D}" name="Hôn nhân" dataDxfId="12"/>
     <tableColumn id="10" xr3:uid="{EF3BB8B0-7D62-4582-84CF-7DC2355334CB}" name="Mức lương (VND)" dataDxfId="11"/>
     <tableColumn id="11" xr3:uid="{828AF2B0-7195-427F-9473-821B448EFACF}" name="Ngày vào làm_x000a_(yyyy-MM-dd) " dataDxfId="10"/>
@@ -1026,7 +1059,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6A2D9191-4CE9-4E69-B805-9A4FDC6A0840}" name="Table3" displayName="Table3" ref="A2:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6A2D9191-4CE9-4E69-B805-9A4FDC6A0840}" name="Table3" displayName="Table3" ref="A2:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A2:C7" xr:uid="{6A2D9191-4CE9-4E69-B805-9A4FDC6A0840}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D2BE2BAF-1CF2-404E-A970-E88DD633B934}" name="STT" dataDxfId="2"/>
@@ -1038,7 +1071,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1337,44 +1370,44 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" customWidth="1"/>
+    <col min="3" max="3" width="14.8984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" customWidth="1"/>
+    <col min="5" max="5" width="15.69921875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" customWidth="1"/>
+    <col min="8" max="8" width="31.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.3984375" customWidth="1"/>
+    <col min="10" max="10" width="17.8984375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.3984375" customWidth="1"/>
+    <col min="13" max="13" width="20.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="43.5" customHeight="1">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-    </row>
-    <row r="2" spans="1:13" ht="30.75" customHeight="1">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+    </row>
+    <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
@@ -1415,11 +1448,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
@@ -1454,15 +1489,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>15</v>
@@ -1471,13 +1506,13 @@
         <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>20</v>
@@ -1495,15 +1530,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>15</v>
@@ -1512,18 +1547,18 @@
         <v>16</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>19</v>
+      <c r="H5" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="I5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="27">
         <v>30000000</v>
       </c>
       <c r="K5" s="26" t="s">
@@ -1532,16 +1567,16 @@
       <c r="L5" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="M5" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>14</v>
@@ -1558,13 +1593,13 @@
       <c r="G6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="27" t="s">
-        <v>19</v>
+      <c r="H6" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="27">
         <v>30000000</v>
       </c>
       <c r="K6" s="26" t="s">
@@ -1573,16 +1608,16 @@
       <c r="L6" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>14</v>
@@ -1599,13 +1634,13 @@
       <c r="G7" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="27" t="s">
-        <v>19</v>
+      <c r="H7" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="27">
         <v>30000000</v>
       </c>
       <c r="K7" s="26" t="s">
@@ -1614,16 +1649,16 @@
       <c r="L7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>6</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>14</v>
@@ -1640,13 +1675,13 @@
       <c r="G8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="27" t="s">
-        <v>19</v>
+      <c r="H8" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="27">
         <v>30000000</v>
       </c>
       <c r="K8" s="26" t="s">
@@ -1655,16 +1690,16 @@
       <c r="L8" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>7</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>14</v>
@@ -1676,18 +1711,18 @@
         <v>16</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="G9" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="27" t="s">
-        <v>19</v>
+      <c r="H9" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I9" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="27">
         <v>30000000</v>
       </c>
       <c r="K9" s="26" t="s">
@@ -1696,16 +1731,16 @@
       <c r="L9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="29" t="s">
+      <c r="M9" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>8</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>14</v>
@@ -1722,13 +1757,13 @@
       <c r="G10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="27" t="s">
-        <v>19</v>
+      <c r="H10" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I10" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="27">
         <v>30000000</v>
       </c>
       <c r="K10" s="26" t="s">
@@ -1737,19 +1772,19 @@
       <c r="L10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>9</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>15</v>
@@ -1763,13 +1798,13 @@
       <c r="G11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="27" t="s">
-        <v>19</v>
+      <c r="H11" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="27">
         <v>30000000</v>
       </c>
       <c r="K11" s="26" t="s">
@@ -1778,16 +1813,16 @@
       <c r="L11" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="29" t="s">
+      <c r="M11" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>10</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>14</v>
@@ -1804,13 +1839,13 @@
       <c r="G12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="27" t="s">
-        <v>19</v>
+      <c r="H12" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I12" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="27">
         <v>30000000</v>
       </c>
       <c r="K12" s="26" t="s">
@@ -1819,16 +1854,16 @@
       <c r="L12" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>11</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>14</v>
@@ -1845,13 +1880,13 @@
       <c r="G13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="27" t="s">
-        <v>19</v>
+      <c r="H13" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="27">
         <v>30000000</v>
       </c>
       <c r="K13" s="26" t="s">
@@ -1860,16 +1895,16 @@
       <c r="L13" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>12</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>14</v>
@@ -1886,13 +1921,13 @@
       <c r="G14" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="27" t="s">
-        <v>19</v>
+      <c r="H14" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="27">
         <v>30000000</v>
       </c>
       <c r="K14" s="26" t="s">
@@ -1901,16 +1936,16 @@
       <c r="L14" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="29" t="s">
+      <c r="M14" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>13</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>14</v>
@@ -1927,13 +1962,13 @@
       <c r="G15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="27" t="s">
-        <v>19</v>
+      <c r="H15" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="27">
         <v>30000000</v>
       </c>
       <c r="K15" s="26" t="s">
@@ -1942,16 +1977,16 @@
       <c r="L15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="29" t="s">
+      <c r="M15" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>14</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>14</v>
@@ -1968,13 +2003,13 @@
       <c r="G16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="27" t="s">
-        <v>19</v>
+      <c r="H16" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I16" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="27">
         <v>30000000</v>
       </c>
       <c r="K16" s="26" t="s">
@@ -1983,16 +2018,16 @@
       <c r="L16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="29" t="s">
+      <c r="M16" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>15</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>14</v>
@@ -2009,13 +2044,13 @@
       <c r="G17" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="27" t="s">
-        <v>19</v>
+      <c r="H17" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I17" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="28">
+      <c r="J17" s="27">
         <v>30000000</v>
       </c>
       <c r="K17" s="26" t="s">
@@ -2024,16 +2059,16 @@
       <c r="L17" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="29" t="s">
+      <c r="M17" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>16</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>14</v>
@@ -2050,13 +2085,13 @@
       <c r="G18" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="27" t="s">
-        <v>19</v>
+      <c r="H18" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="I18" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="27">
         <v>30000000</v>
       </c>
       <c r="K18" s="26" t="s">
@@ -2065,7 +2100,7 @@
       <c r="L18" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="29" t="s">
+      <c r="M18" s="28" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2090,26 +2125,14 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" xr:uid="{CC7C0DCE-74A9-4099-8658-1C9C59A5BD79}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{317F0368-1F8C-4218-9D4C-87951E4D3F14}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{FE5FBDE8-9423-406F-B306-4CD545C705F1}"/>
-    <hyperlink ref="H6" r:id="rId4" xr:uid="{9EA80602-A299-4470-9F9D-5076E529714B}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{474A50C9-01F9-4E32-89EA-D2075307EF19}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{78C6F559-E3E7-4148-9FA2-5FD4035DAD5E}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{FAEFB254-945D-4837-A9FE-699BE2F4CA95}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{E6864FC4-5D10-41DC-82B2-F2873E91CBF1}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{B388EB5B-4615-4E9D-A148-3896021EBF14}"/>
-    <hyperlink ref="H12" r:id="rId10" xr:uid="{F9B60780-20CC-4FCB-BAB1-EE96314D90FC}"/>
-    <hyperlink ref="H13" r:id="rId11" xr:uid="{8D390E52-CAC2-4B14-91FB-46DB2ED2A833}"/>
-    <hyperlink ref="H14" r:id="rId12" xr:uid="{8C31DA5B-A5BB-4256-8CB5-E098E3D5FFB0}"/>
-    <hyperlink ref="H15" r:id="rId13" xr:uid="{63EFB53A-9874-47A9-B3A7-2017DB99EDB4}"/>
-    <hyperlink ref="H16" r:id="rId14" xr:uid="{1ED73EE4-DA0D-4C2D-893B-57881B238855}"/>
-    <hyperlink ref="H17" r:id="rId15" xr:uid="{6265B2A9-8AA5-482E-9297-3160DDA4640B}"/>
-    <hyperlink ref="H18" r:id="rId16" xr:uid="{7C97841D-E862-4985-AEA4-C5C21A281057}"/>
+    <hyperlink ref="H4:H8" r:id="rId2" display="tuan.197pm21936@vanlanguni.vn" xr:uid="{7142461B-9D34-4CA5-8201-90BF45ED052A}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{52D9CD85-88FB-4F8D-B72E-ED44FB0E72E7}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{9E2EC50F-06A3-400D-9310-F4836FC9ED9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2122,54 +2145,54 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.09765625" customWidth="1"/>
+    <col min="2" max="2" width="29.19921875" customWidth="1"/>
+    <col min="3" max="3" width="30.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22.5" customHeight="1">
-      <c r="A1" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="33"/>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1">
+    <row r="1" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -2177,29 +2200,29 @@
         <v>22</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>7</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>